<commit_message>
Updated maps and data cat.
</commit_message>
<xml_diff>
--- a/tables/CSIEM_Data_Catalogue.xlsx
+++ b/tables/CSIEM_Data_Catalogue.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00065525\GITHUB\csiem-data\data-governance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00065525\Github\csiem-data\data-governance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCCA7A7-A5B1-4AD7-976B-19ABF1F8EBCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22942C04-3ED7-486E-A43C-CBE2C60B931B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{BC9683DB-6EDF-419C-90AE-B9006858D13B}"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="28800" windowHeight="15540" xr2:uid="{BC9683DB-6EDF-419C-90AE-B9006858D13B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="130">
   <si>
     <t>Group</t>
   </si>
@@ -418,6 +418,12 @@
   </si>
   <si>
     <t>GK-PAR</t>
+  </si>
+  <si>
+    <t>WWMSP3</t>
+  </si>
+  <si>
+    <t>Ongoing</t>
   </si>
 </sst>
 </file>
@@ -525,21 +531,21 @@
   <dxfs count="2">
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -853,12 +859,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93540D03-D0CE-447B-B6B5-ABD8DB3C1678}">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="555" topLeftCell="A19" activePane="bottomLeft"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="I39" sqref="I39"/>
+      <selection pane="bottomLeft" activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1942,31 +1948,31 @@
         <v>61</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>72</v>
+        <v>26</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>44</v>
+        <v>128</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>116</v>
+        <v>84</v>
+      </c>
+      <c r="H35" s="5">
+        <v>18</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>92</v>
+        <v>129</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -1983,19 +1989,19 @@
         <v>42</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="H36" s="5" t="s">
         <v>116</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>119</v>
@@ -2015,19 +2021,22 @@
         <v>42</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>116</v>
       </c>
+      <c r="I37" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="J37" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -2043,28 +2052,57 @@
       <c r="D38" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E38" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>127</v>
+      <c r="E38" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H38" s="5">
+      <c r="H38" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H39" s="5">
         <v>1</v>
       </c>
-      <c r="I38" s="1" t="s">
+      <c r="I39" s="1" t="s">
         <v>94</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",J1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>